<commit_message>
update website with publication
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ballani5\OneDrive - Novartis Pharma AG\ASA\cgtxwg_webpage\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.novartis.net/personal/ballani5_novartis_net/Documents/ASA/cgtxwg_webpage/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787B0B8F-F502-4DAA-BDE5-71A5006475D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="564" documentId="13_ncr:1_{98D746A2-C07E-4FF5-A27E-62B1DCC3A2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42EF3C04-C1C8-44C7-9B71-02E1A6C62214}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="210" windowWidth="27390" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="1530" windowWidth="22695" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="171">
   <si>
     <t>Index</t>
   </si>
@@ -564,24 +564,6 @@
   </si>
   <si>
     <t>Lead_TF</t>
-  </si>
-  <si>
-    <t>cmc</t>
-  </si>
-  <si>
-    <t>estimand</t>
-  </si>
-  <si>
-    <t>conted</t>
-  </si>
-  <si>
-    <t>dosefinding</t>
-  </si>
-  <si>
-    <t>rwe</t>
-  </si>
-  <si>
-    <t>trialdesign</t>
   </si>
   <si>
     <t>ltfu</t>
@@ -1494,13 +1476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3653B4CE-B4CC-45A0-9176-486D164B59B0}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,8 +1495,7 @@
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="9" max="10" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -1603,7 +1584,7 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
       <c r="J2" s="34" t="s">
-        <v>170</v>
+        <v>38</v>
       </c>
       <c r="K2" s="33"/>
       <c r="L2" s="33"/>
@@ -1962,7 +1943,9 @@
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="34" t="s">
+        <v>170</v>
+      </c>
       <c r="K13" s="33">
         <v>1</v>
       </c>
@@ -2033,7 +2016,7 @@
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
       <c r="J15" s="34" t="s">
-        <v>171</v>
+        <v>18</v>
       </c>
       <c r="K15" s="33"/>
       <c r="L15" s="33">
@@ -2071,7 +2054,7 @@
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
       <c r="J16" s="34" t="s">
-        <v>172</v>
+        <v>70</v>
       </c>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
@@ -2145,7 +2128,7 @@
       <c r="H18" s="33"/>
       <c r="I18" s="33"/>
       <c r="J18" s="34" t="s">
-        <v>173</v>
+        <v>67</v>
       </c>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
@@ -2211,7 +2194,7 @@
       <c r="H20" s="33"/>
       <c r="I20" s="33"/>
       <c r="J20" s="33" t="s">
-        <v>174</v>
+        <v>68</v>
       </c>
       <c r="K20" s="33">
         <v>1</v>
@@ -2232,26 +2215,26 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="C21" s="33"/>
       <c r="D21" s="33" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>163</v>
       </c>
       <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
-        <v>96</v>
+      <c r="G21" s="40" t="s">
+        <v>151</v>
       </c>
       <c r="H21" s="33"/>
       <c r="I21" s="33"/>
-      <c r="J21" s="33" t="s">
-        <v>176</v>
+      <c r="J21" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -2263,29 +2246,23 @@
       <c r="R21" s="33"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>152</v>
-      </c>
+      <c r="A22" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="33"/>
       <c r="C22" s="33"/>
-      <c r="D22" s="33" t="s">
-        <v>159</v>
-      </c>
+      <c r="D22" s="33"/>
       <c r="E22" s="33" t="s">
         <v>163</v>
       </c>
       <c r="F22" s="33"/>
-      <c r="G22" s="40" t="s">
-        <v>151</v>
-      </c>
+      <c r="G22" s="33"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
-      <c r="J22" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="K22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33">
+        <v>1</v>
+      </c>
       <c r="L22" s="33"/>
       <c r="M22" s="33"/>
       <c r="N22" s="33"/>
@@ -2295,24 +2272,32 @@
       <c r="R22" s="33"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
+      <c r="A23" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>160</v>
+      </c>
       <c r="E23" s="33" t="s">
         <v>163</v>
       </c>
       <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="G23" s="33" t="s">
+        <v>100</v>
+      </c>
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
       <c r="J23" s="33"/>
-      <c r="K23" s="33">
-        <v>1</v>
-      </c>
-      <c r="L23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33">
+        <v>1</v>
+      </c>
       <c r="M23" s="33"/>
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
@@ -2322,89 +2307,83 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>162</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C24" s="33"/>
       <c r="D24" s="33" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33">
-        <v>1</v>
-      </c>
+      <c r="K24" s="33">
+        <v>1</v>
+      </c>
+      <c r="L24" s="33"/>
       <c r="M24" s="33"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
+      <c r="Q24" s="33">
+        <v>1</v>
+      </c>
       <c r="R24" s="33"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>138</v>
+      <c r="A25" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>135</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F25" s="33"/>
-      <c r="G25" s="33" t="s">
-        <v>98</v>
+      <c r="G25" s="41" t="s">
+        <v>90</v>
       </c>
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="J25" s="33"/>
-      <c r="K25" s="33">
-        <v>1</v>
-      </c>
+      <c r="K25" s="33"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
-      <c r="Q25" s="33">
-        <v>1</v>
-      </c>
+      <c r="Q25" s="33"/>
       <c r="R25" s="33"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>135</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B26" s="41"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>163</v>
       </c>
       <c r="F26" s="33"/>
       <c r="G26" s="41" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H26" s="33"/>
       <c r="I26" s="33"/>
@@ -2420,19 +2399,21 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="41"/>
+        <v>131</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>132</v>
+      </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>163</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="41" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
@@ -2447,22 +2428,20 @@
       <c r="R27" s="33"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
-        <v>131</v>
-      </c>
+      <c r="A28" s="41"/>
       <c r="B28" s="41" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>163</v>
       </c>
       <c r="F28" s="33"/>
       <c r="G28" s="41" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
@@ -2475,34 +2454,6 @@
       <c r="P28" s="33"/>
       <c r="Q28" s="33"/>
       <c r="R28" s="33"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{3653B4CE-B4CC-45A0-9176-486D164B59B0}"/>
@@ -2521,12 +2472,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
+  <conditionalFormatting sqref="J21">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:R25">
+  <conditionalFormatting sqref="K1:R24">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update objectives and members
</commit_message>
<xml_diff>
--- a/data/members.xlsx
+++ b/data/members.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.novartis.net/sites/ASACGTSWG/Shared Documents/General/ASA_CGT_SWG/cgtxwg_webpage/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="14_{FD9FC8CE-EFE6-4378-BD92-FED0557EEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73FA0DFF-0EFC-4F48-9A1B-B8165899B29F}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="14_{FD9FC8CE-EFE6-4378-BD92-FED0557EEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62F29C6C-570B-4BDF-9C2E-DE4D34361632}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="1260" windowWidth="28275" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="186">
   <si>
     <t>Index</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>DSAI</t>
+  </si>
+  <si>
+    <t>Shen</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>&lt;frank.shen@bms.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1007,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1083,9 +1092,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1102,10 +1108,85 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1115,83 +1196,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1199,7 +1206,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A94E586B-D66C-4475-B46B-862815DB5CEF}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1526,13 +1543,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3653B4CE-B4CC-45A0-9176-486D164B59B0}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,1125 +1575,1173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="44" t="s">
+      <c r="S1" s="40" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33">
-        <v>1</v>
-      </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33">
-        <v>1</v>
-      </c>
-      <c r="S2" s="33">
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32">
+        <v>1</v>
+      </c>
+      <c r="N2" s="32">
+        <v>1</v>
+      </c>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32">
+        <v>1</v>
+      </c>
+      <c r="S2" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33" t="s">
+      <c r="F3" s="32"/>
+      <c r="G3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33">
-        <v>1</v>
-      </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32">
+        <v>1</v>
+      </c>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33">
-        <v>1</v>
-      </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33">
-        <v>1</v>
-      </c>
-      <c r="S4" s="33"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32">
+        <v>1</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32">
+        <v>1</v>
+      </c>
+      <c r="S4" s="32"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="32"/>
+      <c r="G5" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33">
-        <v>1</v>
-      </c>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32">
+        <v>1</v>
+      </c>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33" t="s">
+      <c r="F6" s="32"/>
+      <c r="G6" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33">
-        <v>1</v>
-      </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32">
+        <v>1</v>
+      </c>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33" t="s">
+      <c r="F7" s="32"/>
+      <c r="G7" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33">
-        <v>1</v>
-      </c>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32">
+        <v>1</v>
+      </c>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="s">
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33">
-        <v>1</v>
-      </c>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32">
+        <v>1</v>
+      </c>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33" t="s">
+      <c r="F9" s="32"/>
+      <c r="G9" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33">
-        <v>1</v>
-      </c>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32">
+        <v>1</v>
+      </c>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33" t="s">
+      <c r="F10" s="32"/>
+      <c r="G10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33">
-        <v>1</v>
-      </c>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33">
-        <v>1</v>
-      </c>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33">
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32">
+        <v>1</v>
+      </c>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32">
+        <v>1</v>
+      </c>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33" t="s">
+      <c r="F11" s="32"/>
+      <c r="G11" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33">
-        <v>1</v>
-      </c>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32">
+        <v>1</v>
+      </c>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="32"/>
+      <c r="G12" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33">
-        <v>1</v>
-      </c>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="33"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32">
+        <v>1</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33" t="s">
+      <c r="F13" s="32"/>
+      <c r="G13" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34" t="s">
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="33">
-        <v>1</v>
-      </c>
-      <c r="L13" s="33">
-        <v>1</v>
-      </c>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33"/>
+      <c r="K13" s="32">
+        <v>1</v>
+      </c>
+      <c r="L13" s="32">
+        <v>1</v>
+      </c>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33" t="s">
+      <c r="F14" s="32"/>
+      <c r="G14" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33">
-        <v>1</v>
-      </c>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33">
-        <v>1</v>
-      </c>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32">
+        <v>1</v>
+      </c>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32">
+        <v>1</v>
+      </c>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33" t="s">
+      <c r="F15" s="32"/>
+      <c r="G15" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34" t="s">
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33">
-        <v>1</v>
-      </c>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="33">
-        <v>1</v>
-      </c>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32">
+        <v>1</v>
+      </c>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="32">
+        <v>1</v>
+      </c>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33" t="s">
+      <c r="F16" s="32"/>
+      <c r="G16" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34" t="s">
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="33">
-        <v>1</v>
-      </c>
-      <c r="R16" s="33">
-        <v>1</v>
-      </c>
-      <c r="S16" s="33"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="32">
+        <v>1</v>
+      </c>
+      <c r="R16" s="32">
+        <v>1</v>
+      </c>
+      <c r="S16" s="32"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34" t="s">
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33">
-        <v>1</v>
-      </c>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="33">
-        <v>1</v>
-      </c>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32">
+        <v>1</v>
+      </c>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="32">
+        <v>1</v>
+      </c>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33" t="s">
+      <c r="F18" s="32"/>
+      <c r="G18" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34" t="s">
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33">
-        <v>1</v>
-      </c>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32">
+        <v>1</v>
+      </c>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33" t="s">
+      <c r="F19" s="32"/>
+      <c r="G19" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34" t="s">
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33">
-        <v>1</v>
-      </c>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
-      <c r="S19" s="33"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32">
+        <v>1</v>
+      </c>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33" t="s">
+      <c r="F20" s="32"/>
+      <c r="G20" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34" t="s">
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="K20" s="33">
-        <v>1</v>
-      </c>
-      <c r="L20" s="33">
-        <v>1</v>
-      </c>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33">
-        <v>1</v>
-      </c>
-      <c r="S20" s="33"/>
+      <c r="K20" s="32">
+        <v>1</v>
+      </c>
+      <c r="L20" s="32">
+        <v>1</v>
+      </c>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32">
+        <v>1</v>
+      </c>
+      <c r="S20" s="32"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
+      <c r="F21" s="32"/>
+      <c r="G21" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34" t="s">
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="40" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34" t="s">
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33" t="s">
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="41" t="s">
+      <c r="F23" s="70"/>
+      <c r="G23" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="33">
-        <v>1</v>
-      </c>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="32">
+        <v>1</v>
+      </c>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33" t="s">
+      <c r="F24" s="70"/>
+      <c r="G24" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33">
-        <v>1</v>
-      </c>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32">
+        <v>1</v>
+      </c>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33" t="s">
+      <c r="C25" s="70"/>
+      <c r="D25" s="70" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33" t="s">
+      <c r="F25" s="70"/>
+      <c r="G25" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="33">
-        <v>1</v>
-      </c>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33">
-        <v>1</v>
-      </c>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33">
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="32">
+        <v>1</v>
+      </c>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32">
+        <v>1</v>
+      </c>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33" t="s">
+      <c r="C26" s="70"/>
+      <c r="D26" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="41" t="s">
+      <c r="F26" s="70"/>
+      <c r="G26" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="33"/>
-      <c r="S26" s="33"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33" t="s">
+      <c r="C27" s="70"/>
+      <c r="D27" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="41" t="s">
+      <c r="F27" s="70"/>
+      <c r="G27" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33" t="s">
+      <c r="C28" s="70"/>
+      <c r="D28" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="41" t="s">
+      <c r="F28" s="70"/>
+      <c r="G28" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="33">
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="70" t="s">
         <v>169</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="70" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33" t="s">
+      <c r="C29" s="70"/>
+      <c r="D29" s="70" t="s">
         <v>170</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="41" t="s">
+      <c r="F29" s="70"/>
+      <c r="G29" s="70" t="s">
         <v>172</v>
       </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33">
-        <v>1</v>
-      </c>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="33"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32">
+        <v>1</v>
+      </c>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="70" t="s">
         <v>176</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="70" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="C30" s="70"/>
+      <c r="D30" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="E30" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="G30" s="42" t="s">
+      <c r="F30" s="70"/>
+      <c r="G30" s="70" t="s">
         <v>178</v>
       </c>
-      <c r="J30" t="s">
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="33"/>
-      <c r="S30" s="33">
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="70" t="s">
         <v>179</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="C31" s="70"/>
+      <c r="D31" s="70" t="s">
         <v>173</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="G31" s="42" t="s">
+      <c r="F31" s="70"/>
+      <c r="G31" s="70" t="s">
         <v>181</v>
       </c>
-      <c r="J31" t="s">
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="33"/>
-      <c r="S31" s="33">
-        <v>1</v>
-      </c>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32">
+        <v>1</v>
+      </c>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{3653B4CE-B4CC-45A0-9176-486D164B59B0}"/>
   <conditionalFormatting sqref="J2">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:J18">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15:J18">
+  <conditionalFormatting sqref="J22:J29">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22:J29">
+  <conditionalFormatting sqref="K2:S31">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:S31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="S1 K1:R25">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1 K1:R25">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+  <conditionalFormatting sqref="K32:S32">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3022,46 +3087,46 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
-        <v>1</v>
-      </c>
-      <c r="B2" s="56" t="s">
+      <c r="A2" s="66">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="72" t="s">
+      <c r="H2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="41" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="56"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="52"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -3093,16 +3158,16 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="49">
+      <c r="A5" s="43">
         <v>3</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="49" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="52" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="18" t="s">
@@ -3120,12 +3185,12 @@
       <c r="I5" s="29"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="61"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -3133,12 +3198,12 @@
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="58"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="61"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -3146,12 +3211,12 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="58"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="61"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -3159,12 +3224,12 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -3172,12 +3237,12 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -3212,16 +3277,16 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="49">
+      <c r="A12" s="43">
         <v>5</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="56" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="60"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -3229,12 +3294,12 @@
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="62"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -3242,56 +3307,56 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="48">
+      <c r="A14" s="66">
         <v>6</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="48" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="70" t="s">
+      <c r="H14" s="62" t="s">
         <v>51</v>
       </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="71"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="63"/>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49">
+      <c r="A16" s="43">
         <v>7</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="58" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="41" t="s">
         <v>55</v>
       </c>
       <c r="E16" s="22" t="s">
@@ -3311,12 +3376,12 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="67"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="61"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -3326,12 +3391,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="68"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="52"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="25"/>
@@ -3382,6 +3447,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A5:A10"/>
@@ -3398,14 +3471,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3413,15 +3478,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100783019AEDAA863499A5FE548DC86AC7C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31ec6b447407bce11483c535c98261eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="238314b5-2e5b-4df7-a1a7-303d49bb0d3d" xmlns:ns3="13d981ae-15aa-45ba-ad30-ef48ef224202" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efb08ee3d2dc06d7ab1aa189987b284f" ns2:_="" ns3:_="">
     <xsd:import namespace="238314b5-2e5b-4df7-a1a7-303d49bb0d3d"/>
@@ -3644,15 +3700,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E175666-8B1F-4390-B4F7-61AAE2C63967}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AED2D26-97CB-4E51-A754-E03BB320F0B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3669,4 +3726,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E175666-8B1F-4390-B4F7-61AAE2C63967}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>